<commit_message>
Push ITwork briefing for review Signed-off-by: Tetsumaro <s3923443@student.rmit.edu.au>
</commit_message>
<xml_diff>
--- a/Tools/Excels - Project Plan Management/Assigment 2 - Planning - 20211014-20211017-Agreed.xlsx
+++ b/Tools/Excels - Project Plan Management/Assigment 2 - Planning - 20211014-20211017-Agreed.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tetsu Watanabe\github\stockIT\Tools\Project Plan Management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tetsu Watanabe\github\stockIT\Tools\Excels - Project Plan Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DECF72D-A335-46DF-AE66-1AA68EC94F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDAAF9A-8D9C-4BE4-BF5B-6D747B03C779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4CDF8357-69BB-4CEA-B86F-4958E579877B}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4CDF8357-69BB-4CEA-B86F-4958E579877B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -249,7 +249,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -286,6 +286,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -453,15 +459,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -480,84 +483,93 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -567,13 +579,25 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -893,40 +917,40 @@
   <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A24" zoomScale="60" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O41" sqref="O41"/>
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" style="6" customWidth="1"/>
     <col min="6" max="9" width="9.140625" style="1"/>
     <col min="10" max="10" width="0" style="1" hidden="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="40" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="36" t="s">
         <v>38</v>
       </c>
       <c r="J2" s="1" t="s">
@@ -934,17 +958,17 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+      <c r="A3" s="46">
         <v>1</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17" t="s">
+      <c r="C3" s="44"/>
+      <c r="D3" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="45" t="s">
         <v>49</v>
       </c>
       <c r="J3" s="1" t="s">
@@ -952,17 +976,17 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+      <c r="A4" s="47">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
+      <c r="C4" s="42"/>
+      <c r="D4" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="43" t="s">
         <v>53</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -970,17 +994,17 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="17" t="s">
         <v>55</v>
       </c>
       <c r="J5" s="1" t="s">
@@ -988,17 +1012,17 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="17" t="s">
         <v>56</v>
       </c>
       <c r="J6" s="1" t="s">
@@ -1006,17 +1030,17 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="19" t="s">
+      <c r="C7" s="42"/>
+      <c r="D7" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="43" t="s">
         <v>52</v>
       </c>
       <c r="J7" s="1" t="s">
@@ -1024,440 +1048,440 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="117.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20" t="s">
+      <c r="C8" s="18"/>
+      <c r="D8" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="19" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>1</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17" t="s">
+      <c r="C10" s="15"/>
+      <c r="D10" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="16" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
+      <c r="A11" s="14">
         <v>2</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22" t="s">
+      <c r="C11" s="20"/>
+      <c r="D11" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="21" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="7">
         <v>1</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24" t="s">
+      <c r="C14" s="22"/>
+      <c r="D14" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="23" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15">
+      <c r="A17" s="13">
         <v>1</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26" t="s">
+      <c r="C17" s="24"/>
+      <c r="D17" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="27" t="s">
+      <c r="E17" s="25" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
+      <c r="A20" s="7">
         <v>1</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24" t="s">
+      <c r="C20" s="22"/>
+      <c r="D20" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="25" t="s">
+      <c r="E20" s="23" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="13">
+      <c r="A23" s="11">
         <v>1</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28" t="s">
+      <c r="C23" s="26"/>
+      <c r="D23" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="29" t="s">
+      <c r="E23" s="27" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="14">
+      <c r="A24" s="12">
         <v>2</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30" t="s">
+      <c r="C24" s="28"/>
+      <c r="D24" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="31" t="s">
+      <c r="E24" s="29" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="9">
+      <c r="A25" s="8">
         <v>3</v>
       </c>
-      <c r="B25" s="32" t="s">
+      <c r="B25" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32" t="s">
+      <c r="C25" s="30"/>
+      <c r="D25" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="33" t="s">
+      <c r="E25" s="31" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="9">
+      <c r="A26" s="8">
         <v>4</v>
       </c>
-      <c r="B26" s="32" t="s">
+      <c r="B26" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32" t="s">
+      <c r="C26" s="30"/>
+      <c r="D26" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="33" t="s">
+      <c r="E26" s="31" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="9">
+      <c r="A27" s="8">
         <v>5</v>
       </c>
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32" t="s">
+      <c r="C27" s="30"/>
+      <c r="D27" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="33" t="s">
+      <c r="E27" s="31" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="11">
+      <c r="A28" s="9">
         <v>6</v>
       </c>
-      <c r="B28" s="34" t="s">
+      <c r="B28" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="35"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="33"/>
     </row>
     <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="4">
+      <c r="A31" s="3">
         <v>1</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E31" s="18" t="s">
+      <c r="C31" s="44"/>
+      <c r="D31" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="45" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="5">
+      <c r="A32" s="4">
         <v>2</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E32" s="19" t="s">
+      <c r="C32" s="2"/>
+      <c r="D32" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" s="17" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="5">
+      <c r="A33" s="4">
         <v>3</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E33" s="19" t="s">
+      <c r="C33" s="2"/>
+      <c r="D33" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33" s="17" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="5">
+      <c r="A34" s="4">
         <v>4</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E34" s="19" t="s">
+      <c r="C34" s="2"/>
+      <c r="D34" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E34" s="17" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="5">
+      <c r="A35" s="4">
         <v>5</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E35" s="19" t="s">
+      <c r="C35" s="2"/>
+      <c r="D35" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" s="17" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="5">
+      <c r="A36" s="4">
         <v>6</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E36" s="19" t="s">
+      <c r="C36" s="2"/>
+      <c r="D36" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36" s="17" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="5">
+      <c r="A37" s="4">
         <v>7</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E37" s="19" t="s">
+      <c r="C37" s="2"/>
+      <c r="D37" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E37" s="17" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="5">
+      <c r="A38" s="4">
         <v>8</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E38" s="19" t="s">
+      <c r="C38" s="2"/>
+      <c r="D38" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38" s="17" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="5">
+      <c r="A39" s="4">
         <v>9</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E39" s="19" t="s">
+      <c r="C39" s="2"/>
+      <c r="D39" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E39" s="17" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="5">
+      <c r="A40" s="4">
         <v>6</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E40" s="19" t="s">
+      <c r="C40" s="42"/>
+      <c r="D40" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E40" s="43" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="10">
+      <c r="A41" s="37">
         <v>7</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E41" s="19" t="s">
+      <c r="C41" s="42"/>
+      <c r="D41" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E41" s="43" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="3" t="s">
+      <c r="A42" s="37"/>
+      <c r="B42" s="41"/>
+      <c r="C42" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E42" s="19" t="s">
+      <c r="D42" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E42" s="43" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="10"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="3" t="s">
+      <c r="A43" s="37"/>
+      <c r="B43" s="41"/>
+      <c r="C43" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E43" s="19" t="s">
+      <c r="D43" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E43" s="43" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A44" s="10"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="3" t="s">
+      <c r="A44" s="37"/>
+      <c r="B44" s="41"/>
+      <c r="C44" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E44" s="19" t="s">
+      <c r="D44" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E44" s="43" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A45" s="10"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="3" t="s">
+      <c r="A45" s="37"/>
+      <c r="B45" s="41"/>
+      <c r="C45" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E45" s="19" t="s">
+      <c r="D45" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E45" s="43" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="6">
+      <c r="A46" s="5">
         <v>8</v>
       </c>
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E46" s="21" t="s">
+      <c r="C46" s="18"/>
+      <c r="D46" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E46" s="19" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Push our current project status Signed-off-by: Tetsumaro <s3923443@student.rmit.edu.au>
</commit_message>
<xml_diff>
--- a/Tools/Excels - Project Plan Management/Assigment 2 - Planning - 20211014-20211017-Agreed.xlsx
+++ b/Tools/Excels - Project Plan Management/Assigment 2 - Planning - 20211014-20211017-Agreed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tetsu Watanabe\github\stockIT\Tools\Excels - Project Plan Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDAAF9A-8D9C-4BE4-BF5B-6D747B03C779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E941E1FC-98E5-4BB0-BD23-EE6DDED00B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4CDF8357-69BB-4CEA-B86F-4958E579877B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4CDF8357-69BB-4CEA-B86F-4958E579877B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -249,7 +249,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -282,12 +282,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -459,15 +453,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -477,9 +468,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -489,115 +477,85 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -916,41 +874,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF00C70F-175F-4A72-A368-1206640C5405}">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A24" zoomScale="60" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" style="5" customWidth="1"/>
     <col min="6" max="9" width="9.140625" style="1"/>
     <col min="10" max="10" width="0" style="1" hidden="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="40"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="29"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="35" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="18" t="s">
         <v>38</v>
       </c>
       <c r="J2" s="1" t="s">
@@ -958,17 +916,17 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="46">
+      <c r="A3" s="23">
         <v>1</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44" t="s">
+      <c r="C3" s="21"/>
+      <c r="D3" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="22" t="s">
         <v>49</v>
       </c>
       <c r="J3" s="1" t="s">
@@ -976,17 +934,17 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="47">
+      <c r="A4" s="24">
         <v>2</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42" t="s">
+      <c r="C4" s="19"/>
+      <c r="D4" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="43" t="s">
+      <c r="E4" s="20" t="s">
         <v>53</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -994,7 +952,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1004,7 +962,7 @@
       <c r="D5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="9" t="s">
         <v>55</v>
       </c>
       <c r="J5" s="1" t="s">
@@ -1012,17 +970,17 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+      <c r="A6" s="24">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="19"/>
+      <c r="D6" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="20" t="s">
         <v>56</v>
       </c>
       <c r="J6" s="1" t="s">
@@ -1030,17 +988,17 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
+      <c r="A7" s="24">
         <v>5</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="43" t="s">
+      <c r="C7" s="19"/>
+      <c r="D7" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="20" t="s">
         <v>52</v>
       </c>
       <c r="J7" s="1" t="s">
@@ -1048,258 +1006,258 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="117.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="11" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+      <c r="A10" s="23">
         <v>1</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15" t="s">
+      <c r="C10" s="21"/>
+      <c r="D10" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="22" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
+      <c r="A11" s="33">
         <v>2</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20" t="s">
+      <c r="C11" s="34"/>
+      <c r="D11" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="35" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+      <c r="A14" s="30">
         <v>1</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22" t="s">
+      <c r="C14" s="31"/>
+      <c r="D14" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="32" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13">
+      <c r="A17" s="30">
         <v>1</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24" t="s">
+      <c r="C17" s="31"/>
+      <c r="D17" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="32" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+      <c r="A20" s="30">
         <v>1</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22" t="s">
+      <c r="C20" s="31"/>
+      <c r="D20" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="23" t="s">
+      <c r="E20" s="32" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+    <row r="22" spans="1:5" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="11">
+      <c r="A23" s="23">
         <v>1</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26" t="s">
+      <c r="C23" s="21"/>
+      <c r="D23" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="22" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="12">
+      <c r="A24" s="24">
         <v>2</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28" t="s">
+      <c r="C24" s="19"/>
+      <c r="D24" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="29" t="s">
+      <c r="E24" s="20" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="8">
+      <c r="A25" s="24">
         <v>3</v>
       </c>
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30" t="s">
+      <c r="C25" s="19"/>
+      <c r="D25" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="20" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="8">
+      <c r="A26" s="6">
         <v>4</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30" t="s">
+      <c r="C26" s="12"/>
+      <c r="D26" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="31" t="s">
+      <c r="E26" s="13" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="8">
+      <c r="A27" s="24">
         <v>5</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30" t="s">
+      <c r="C27" s="19"/>
+      <c r="D27" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="31" t="s">
+      <c r="E27" s="20" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="9">
+      <c r="A28" s="7">
         <v>6</v>
       </c>
-      <c r="B28" s="32" t="s">
+      <c r="B28" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="33"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="15"/>
     </row>
     <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3">
+      <c r="A31" s="23">
         <v>1</v>
       </c>
-      <c r="B31" s="44" t="s">
+      <c r="B31" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="44"/>
-      <c r="D31" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="E31" s="45" t="s">
+      <c r="C31" s="21"/>
+      <c r="D31" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="22" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="4">
+      <c r="A32" s="24">
         <v>2</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E32" s="17" t="s">
+      <c r="C32" s="19"/>
+      <c r="D32" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" s="20" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="4">
+      <c r="A33" s="24">
         <v>3</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E33" s="17" t="s">
+      <c r="C33" s="19"/>
+      <c r="D33" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33" s="20" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="4">
+      <c r="A34" s="3">
         <v>4</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -1309,12 +1267,12 @@
       <c r="D34" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E34" s="17" t="s">
+      <c r="E34" s="9" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="4">
+      <c r="A35" s="3">
         <v>5</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -1324,12 +1282,12 @@
       <c r="D35" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="17" t="s">
+      <c r="E35" s="9" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="4">
+      <c r="A36" s="3">
         <v>6</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -1339,12 +1297,12 @@
       <c r="D36" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E36" s="17" t="s">
+      <c r="E36" s="9" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="4">
+      <c r="A37" s="3">
         <v>7</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -1354,12 +1312,12 @@
       <c r="D37" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E37" s="17" t="s">
+      <c r="E37" s="9" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="4">
+      <c r="A38" s="3">
         <v>8</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -1369,12 +1327,12 @@
       <c r="D38" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E38" s="17" t="s">
+      <c r="E38" s="9" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="4">
+      <c r="A39" s="3">
         <v>9</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -1384,104 +1342,104 @@
       <c r="D39" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E39" s="17" t="s">
+      <c r="E39" s="9" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="4">
+      <c r="A40" s="3">
         <v>6</v>
       </c>
-      <c r="B40" s="42" t="s">
+      <c r="B40" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="42"/>
-      <c r="D40" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="E40" s="43" t="s">
+      <c r="C40" s="19"/>
+      <c r="D40" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E40" s="20" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="37">
+      <c r="A41" s="26">
         <v>7</v>
       </c>
-      <c r="B41" s="41" t="s">
+      <c r="B41" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="42"/>
-      <c r="D41" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="E41" s="43" t="s">
+      <c r="C41" s="19"/>
+      <c r="D41" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E41" s="20" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="37"/>
-      <c r="B42" s="41"/>
-      <c r="C42" s="42" t="s">
+      <c r="A42" s="26"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D42" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="E42" s="43" t="s">
+      <c r="D42" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E42" s="20" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="37"/>
-      <c r="B43" s="41"/>
-      <c r="C43" s="42" t="s">
+      <c r="A43" s="26"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D43" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="E43" s="43" t="s">
+      <c r="D43" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E43" s="20" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A44" s="37"/>
-      <c r="B44" s="41"/>
-      <c r="C44" s="42" t="s">
+      <c r="A44" s="26"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D44" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="E44" s="43" t="s">
+      <c r="D44" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E44" s="20" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A45" s="37"/>
-      <c r="B45" s="41"/>
-      <c r="C45" s="42" t="s">
+      <c r="A45" s="26"/>
+      <c r="B45" s="25"/>
+      <c r="C45" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D45" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="E45" s="43" t="s">
+      <c r="D45" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E45" s="20" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="5">
+      <c r="A46" s="4">
         <v>8</v>
       </c>
-      <c r="B46" s="18" t="s">
+      <c r="B46" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E46" s="19" t="s">
+      <c r="C46" s="10"/>
+      <c r="D46" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E46" s="11" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>